<commit_message>
i am added some content on myexcel.xlsx
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -11,8 +11,22 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Serial-No</t>
+  </si>
+  <si>
+    <t>Emp-id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,12 +356,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
now i have added some contain myexcel.xlsx to .gitignore
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Serial-No</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>paddy</t>
+  </si>
+  <si>
+    <t>babby</t>
   </si>
 </sst>
 </file>
@@ -362,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -401,6 +404,17 @@
       </c>
       <c r="C3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>